<commit_message>
datos ajustados de metricas para carregar no looker
</commit_message>
<xml_diff>
--- a/metrics/metricas_analysis.xlsx
+++ b/metrics/metricas_analysis.xlsx
@@ -486,16 +486,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1425</v>
+        <v>1236</v>
       </c>
       <c r="C2" t="n">
-        <v>302</v>
+        <v>323</v>
       </c>
       <c r="D2" t="n">
-        <v>666</v>
+        <v>529</v>
       </c>
       <c r="E2" t="n">
-        <v>457</v>
+        <v>384</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -581,7 +581,7 @@
         <v>15.45</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
@@ -671,31 +671,31 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>10390</v>
+        <v>10520</v>
       </c>
       <c r="C7" t="n">
-        <v>1857</v>
+        <v>2029</v>
       </c>
       <c r="D7" t="n">
-        <v>286</v>
+        <v>268</v>
       </c>
       <c r="E7" t="n">
-        <v>1114</v>
+        <v>1145</v>
       </c>
       <c r="F7" t="n">
-        <v>7133</v>
+        <v>7078</v>
       </c>
       <c r="G7" t="n">
-        <v>26.97</v>
+        <v>27</v>
       </c>
       <c r="H7" t="n">
-        <v>5.34</v>
+        <v>5.35</v>
       </c>
       <c r="I7" t="n">
+        <v>13</v>
+      </c>
+      <c r="J7" t="n">
         <v>10</v>
-      </c>
-      <c r="J7" t="n">
-        <v>8</v>
       </c>
       <c r="K7" t="n">
         <v>7</v>
@@ -708,13 +708,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>20234</v>
+        <v>20248</v>
       </c>
       <c r="C8" t="n">
-        <v>1174</v>
+        <v>1204</v>
       </c>
       <c r="D8" t="n">
-        <v>514</v>
+        <v>498</v>
       </c>
       <c r="E8" t="n">
         <v>2507</v>
@@ -729,7 +729,7 @@
         <v>2.28</v>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J8" t="n">
         <v>9</v>
@@ -760,10 +760,10 @@
         <v>14446</v>
       </c>
       <c r="G9" t="n">
-        <v>17.53</v>
+        <v>18.17</v>
       </c>
       <c r="H9" t="n">
-        <v>14.42</v>
+        <v>14.9</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -772,7 +772,7 @@
         <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -782,10 +782,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>6210</v>
+        <v>6422</v>
       </c>
       <c r="C10" t="n">
-        <v>3248</v>
+        <v>3460</v>
       </c>
       <c r="D10" t="n">
         <v>403</v>
@@ -797,10 +797,10 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>10.09</v>
+        <v>10.34</v>
       </c>
       <c r="H10" t="n">
-        <v>4.89</v>
+        <v>4.44</v>
       </c>
       <c r="I10" t="n">
         <v>2</v>
@@ -856,34 +856,34 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>10941</v>
+        <v>11030</v>
       </c>
       <c r="C12" t="n">
-        <v>1571</v>
+        <v>1675</v>
       </c>
       <c r="D12" t="n">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="E12" t="n">
-        <v>1641</v>
+        <v>1648</v>
       </c>
       <c r="F12" t="n">
-        <v>7286</v>
+        <v>7273</v>
       </c>
       <c r="G12" t="n">
-        <v>13.54</v>
+        <v>13.61</v>
       </c>
       <c r="H12" t="n">
-        <v>6.99</v>
+        <v>6.88</v>
       </c>
       <c r="I12" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="J12" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
@@ -920,7 +920,7 @@
         <v>2</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14">
@@ -930,25 +930,25 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>9261</v>
+        <v>9167</v>
       </c>
       <c r="C14" t="n">
-        <v>765</v>
+        <v>775</v>
       </c>
       <c r="D14" t="n">
-        <v>464</v>
+        <v>396</v>
       </c>
       <c r="E14" t="n">
-        <v>809</v>
+        <v>772</v>
       </c>
       <c r="F14" t="n">
         <v>7223</v>
       </c>
       <c r="G14" t="n">
-        <v>11.5</v>
+        <v>11.82</v>
       </c>
       <c r="H14" t="n">
-        <v>10.45</v>
+        <v>10.69</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
@@ -994,7 +994,7 @@
         <v>6</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1080,25 +1080,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2901</v>
+        <v>19716</v>
       </c>
       <c r="C2" t="n">
-        <v>688</v>
+        <v>568</v>
       </c>
       <c r="D2" t="n">
-        <v>110</v>
+        <v>425</v>
       </c>
       <c r="E2" t="n">
-        <v>2103</v>
+        <v>1111</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>17612</v>
       </c>
       <c r="G2" t="n">
-        <v>6.15</v>
+        <v>13.48</v>
       </c>
       <c r="H2" t="n">
-        <v>13.68</v>
+        <v>15.68</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -1107,7 +1107,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -1117,25 +1117,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>15139</v>
+        <v>13577</v>
       </c>
       <c r="C3" t="n">
-        <v>2942</v>
+        <v>2732</v>
       </c>
       <c r="D3" t="n">
-        <v>314</v>
+        <v>636</v>
       </c>
       <c r="E3" t="n">
-        <v>2327</v>
+        <v>2326</v>
       </c>
       <c r="F3" t="n">
-        <v>9556</v>
+        <v>7883</v>
       </c>
       <c r="G3" t="n">
-        <v>9.1</v>
+        <v>8.02</v>
       </c>
       <c r="H3" t="n">
-        <v>2.62</v>
+        <v>6.11</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -1144,7 +1144,7 @@
         <v>5</v>
       </c>
       <c r="K3" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -1154,31 +1154,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7485</v>
+        <v>7823</v>
       </c>
       <c r="C4" t="n">
-        <v>655</v>
+        <v>542</v>
       </c>
       <c r="D4" t="n">
-        <v>24</v>
+        <v>321</v>
       </c>
       <c r="E4" t="n">
-        <v>822</v>
+        <v>976</v>
       </c>
       <c r="F4" t="n">
         <v>5984</v>
       </c>
       <c r="G4" t="n">
-        <v>4.73</v>
+        <v>8.359999999999999</v>
       </c>
       <c r="H4" t="n">
-        <v>3.07</v>
+        <v>6.77</v>
       </c>
       <c r="I4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K4" t="n">
         <v>6</v>
@@ -1191,25 +1191,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4750</v>
+        <v>25013</v>
       </c>
       <c r="C5" t="n">
-        <v>168</v>
+        <v>187</v>
       </c>
       <c r="D5" t="n">
-        <v>1612</v>
+        <v>1342</v>
       </c>
       <c r="E5" t="n">
-        <v>2970</v>
+        <v>2814</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>20670</v>
       </c>
       <c r="G5" t="n">
-        <v>20.3</v>
+        <v>20.68</v>
       </c>
       <c r="H5" t="n">
-        <v>22.16</v>
+        <v>21.73</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -1218,7 +1218,7 @@
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -1228,25 +1228,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>12990</v>
+        <v>13541</v>
       </c>
       <c r="C6" t="n">
-        <v>181</v>
+        <v>322</v>
       </c>
       <c r="D6" t="n">
-        <v>138</v>
+        <v>523</v>
       </c>
       <c r="E6" t="n">
-        <v>1726</v>
+        <v>1751</v>
       </c>
       <c r="F6" t="n">
         <v>10945</v>
       </c>
       <c r="G6" t="n">
-        <v>2.52</v>
+        <v>3.97</v>
       </c>
       <c r="H6" t="n">
-        <v>8.5</v>
+        <v>5.35</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
@@ -1255,7 +1255,7 @@
         <v>8</v>
       </c>
       <c r="K6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -1265,34 +1265,34 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>10675</v>
+        <v>10149</v>
       </c>
       <c r="C7" t="n">
-        <v>1970</v>
+        <v>2003</v>
       </c>
       <c r="D7" t="n">
-        <v>532</v>
+        <v>726</v>
       </c>
       <c r="E7" t="n">
-        <v>542</v>
+        <v>1146</v>
       </c>
       <c r="F7" t="n">
-        <v>7631</v>
+        <v>6274</v>
       </c>
       <c r="G7" t="n">
-        <v>12.52</v>
+        <v>24.02</v>
       </c>
       <c r="H7" t="n">
-        <v>5.58</v>
+        <v>8.869999999999999</v>
       </c>
       <c r="I7" t="n">
+        <v>18</v>
+      </c>
+      <c r="J7" t="n">
         <v>13</v>
       </c>
-      <c r="J7" t="n">
-        <v>11</v>
-      </c>
       <c r="K7" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -1302,28 +1302,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>13357</v>
+        <v>13963</v>
       </c>
       <c r="C8" t="n">
-        <v>1710</v>
+        <v>1852</v>
       </c>
       <c r="D8" t="n">
-        <v>524</v>
+        <v>825</v>
       </c>
       <c r="E8" t="n">
-        <v>1210</v>
+        <v>1293</v>
       </c>
       <c r="F8" t="n">
-        <v>9913</v>
+        <v>9993</v>
       </c>
       <c r="G8" t="n">
-        <v>9.1</v>
+        <v>9.880000000000001</v>
       </c>
       <c r="H8" t="n">
-        <v>16.06</v>
+        <v>13.37</v>
       </c>
       <c r="I8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J8" t="n">
         <v>9</v>
@@ -1339,25 +1339,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17035</v>
+        <v>16423</v>
       </c>
       <c r="C9" t="n">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D9" t="n">
-        <v>99</v>
+        <v>313</v>
       </c>
       <c r="E9" t="n">
-        <v>667</v>
+        <v>622</v>
       </c>
       <c r="F9" t="n">
-        <v>16148</v>
+        <v>15361</v>
       </c>
       <c r="G9" t="n">
-        <v>15.81</v>
+        <v>18.86</v>
       </c>
       <c r="H9" t="n">
-        <v>7.34</v>
+        <v>5.6</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -1366,7 +1366,7 @@
         <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -1376,34 +1376,34 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3135</v>
+        <v>2653</v>
       </c>
       <c r="C10" t="n">
-        <v>1033</v>
+        <v>894</v>
       </c>
       <c r="D10" t="n">
-        <v>572</v>
+        <v>370</v>
       </c>
       <c r="E10" t="n">
-        <v>1530</v>
+        <v>1389</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>3.73</v>
+        <v>4.72</v>
       </c>
       <c r="H10" t="n">
-        <v>1.61</v>
+        <v>3.37</v>
       </c>
       <c r="I10" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="J10" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K10" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -1413,25 +1413,25 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>8643</v>
+        <v>15789</v>
       </c>
       <c r="C11" t="n">
-        <v>543</v>
+        <v>563</v>
       </c>
       <c r="D11" t="n">
-        <v>90</v>
+        <v>247</v>
       </c>
       <c r="E11" t="n">
-        <v>513</v>
+        <v>696</v>
       </c>
       <c r="F11" t="n">
-        <v>7497</v>
+        <v>14283</v>
       </c>
       <c r="G11" t="n">
-        <v>9.01</v>
+        <v>13.42</v>
       </c>
       <c r="H11" t="n">
-        <v>5.19</v>
+        <v>12.94</v>
       </c>
       <c r="I11" t="n">
         <v>5</v>
@@ -1440,7 +1440,7 @@
         <v>9</v>
       </c>
       <c r="K11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -1450,34 +1450,34 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>8663</v>
+        <v>8647</v>
       </c>
       <c r="C12" t="n">
-        <v>1342</v>
+        <v>1322</v>
       </c>
       <c r="D12" t="n">
-        <v>413</v>
+        <v>560</v>
       </c>
       <c r="E12" t="n">
-        <v>1026</v>
+        <v>1201</v>
       </c>
       <c r="F12" t="n">
-        <v>5882</v>
+        <v>5562</v>
       </c>
       <c r="G12" t="n">
-        <v>7.52</v>
+        <v>11.74</v>
       </c>
       <c r="H12" t="n">
-        <v>6.58</v>
+        <v>8.1</v>
       </c>
       <c r="I12" t="n">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J12" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13">
@@ -1487,25 +1487,25 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>8794</v>
+        <v>18114</v>
       </c>
       <c r="C13" t="n">
-        <v>297</v>
+        <v>357</v>
       </c>
       <c r="D13" t="n">
-        <v>613</v>
+        <v>704</v>
       </c>
       <c r="E13" t="n">
-        <v>1736</v>
+        <v>1753</v>
       </c>
       <c r="F13" t="n">
-        <v>6147</v>
+        <v>15299</v>
       </c>
       <c r="G13" t="n">
-        <v>10.61</v>
+        <v>12.69</v>
       </c>
       <c r="H13" t="n">
-        <v>11.95</v>
+        <v>13.34</v>
       </c>
       <c r="I13" t="n">
         <v>6</v>
@@ -1514,7 +1514,7 @@
         <v>17</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -1524,25 +1524,25 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>9968</v>
+        <v>18069</v>
       </c>
       <c r="C14" t="n">
-        <v>404</v>
+        <v>347</v>
       </c>
       <c r="D14" t="n">
-        <v>104</v>
+        <v>369</v>
       </c>
       <c r="E14" t="n">
-        <v>1385</v>
+        <v>866</v>
       </c>
       <c r="F14" t="n">
-        <v>8074</v>
+        <v>16486</v>
       </c>
       <c r="G14" t="n">
-        <v>10.98</v>
+        <v>16.17</v>
       </c>
       <c r="H14" t="n">
-        <v>10.5</v>
+        <v>10.64</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
@@ -1551,7 +1551,7 @@
         <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
@@ -1561,25 +1561,25 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>15139</v>
+        <v>13577</v>
       </c>
       <c r="C15" t="n">
-        <v>2942</v>
+        <v>2732</v>
       </c>
       <c r="D15" t="n">
-        <v>314</v>
+        <v>636</v>
       </c>
       <c r="E15" t="n">
-        <v>2327</v>
+        <v>2326</v>
       </c>
       <c r="F15" t="n">
-        <v>9556</v>
+        <v>7883</v>
       </c>
       <c r="G15" t="n">
-        <v>9.1</v>
+        <v>8.02</v>
       </c>
       <c r="H15" t="n">
-        <v>2.62</v>
+        <v>6.1</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -1588,7 +1588,7 @@
         <v>5</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
criando as metricas de personas
</commit_message>
<xml_diff>
--- a/metrics/metricas_analysis.xlsx
+++ b/metrics/metricas_analysis.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enero" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Febrero" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Febrero" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Marzo" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -486,25 +486,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1236</v>
+        <v>20207</v>
       </c>
       <c r="C2" t="n">
-        <v>323</v>
+        <v>748</v>
       </c>
       <c r="D2" t="n">
-        <v>529</v>
+        <v>470</v>
       </c>
       <c r="E2" t="n">
-        <v>384</v>
+        <v>1377</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>17612</v>
       </c>
       <c r="G2" t="n">
-        <v>5.47</v>
+        <v>16.28</v>
       </c>
       <c r="H2" t="n">
-        <v>6.5</v>
+        <v>18.05</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -513,7 +513,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -523,34 +523,34 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>12618</v>
+        <v>14599</v>
       </c>
       <c r="C3" t="n">
-        <v>1875</v>
+        <v>2857</v>
       </c>
       <c r="D3" t="n">
-        <v>697</v>
+        <v>636</v>
       </c>
       <c r="E3" t="n">
-        <v>411</v>
+        <v>3186</v>
       </c>
       <c r="F3" t="n">
-        <v>9635</v>
+        <v>7920</v>
       </c>
       <c r="G3" t="n">
-        <v>20.27</v>
+        <v>7.69</v>
       </c>
       <c r="H3" t="n">
-        <v>1.1</v>
+        <v>5.74</v>
       </c>
       <c r="I3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -560,34 +560,34 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6932</v>
+        <v>7823</v>
       </c>
       <c r="C4" t="n">
-        <v>8</v>
+        <v>542</v>
       </c>
       <c r="D4" t="n">
-        <v>565</v>
+        <v>321</v>
       </c>
       <c r="E4" t="n">
-        <v>384</v>
+        <v>976</v>
       </c>
       <c r="F4" t="n">
-        <v>5975</v>
+        <v>5984</v>
       </c>
       <c r="G4" t="n">
-        <v>2.62</v>
+        <v>8.359999999999999</v>
       </c>
       <c r="H4" t="n">
-        <v>15.45</v>
+        <v>6.77</v>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -597,25 +597,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>20256</v>
+        <v>25013</v>
       </c>
       <c r="C5" t="n">
-        <v>890</v>
+        <v>187</v>
       </c>
       <c r="D5" t="n">
-        <v>922</v>
+        <v>1342</v>
       </c>
       <c r="E5" t="n">
-        <v>1639</v>
+        <v>2814</v>
       </c>
       <c r="F5" t="n">
-        <v>16805</v>
+        <v>20670</v>
       </c>
       <c r="G5" t="n">
-        <v>8.58</v>
+        <v>20.64</v>
       </c>
       <c r="H5" t="n">
-        <v>3.36</v>
+        <v>21.9</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -624,7 +624,7 @@
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -634,34 +634,34 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>10843</v>
+        <v>13541</v>
       </c>
       <c r="C6" t="n">
-        <v>349</v>
+        <v>322</v>
       </c>
       <c r="D6" t="n">
-        <v>359</v>
+        <v>523</v>
       </c>
       <c r="E6" t="n">
-        <v>777</v>
+        <v>1751</v>
       </c>
       <c r="F6" t="n">
-        <v>9358</v>
+        <v>10945</v>
       </c>
       <c r="G6" t="n">
-        <v>11.7</v>
+        <v>3.97</v>
       </c>
       <c r="H6" t="n">
-        <v>6.23</v>
+        <v>5.35</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K6" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -671,34 +671,34 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>10520</v>
+        <v>10824</v>
       </c>
       <c r="C7" t="n">
-        <v>2029</v>
+        <v>1947</v>
       </c>
       <c r="D7" t="n">
-        <v>268</v>
+        <v>681</v>
       </c>
       <c r="E7" t="n">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="F7" t="n">
-        <v>7078</v>
+        <v>7050</v>
       </c>
       <c r="G7" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H7" t="n">
-        <v>5.35</v>
+        <v>9.25</v>
       </c>
       <c r="I7" t="n">
+        <v>18</v>
+      </c>
+      <c r="J7" t="n">
         <v>13</v>
       </c>
-      <c r="J7" t="n">
-        <v>10</v>
-      </c>
       <c r="K7" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -708,34 +708,34 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>20248</v>
+        <v>13533</v>
       </c>
       <c r="C8" t="n">
-        <v>1204</v>
+        <v>1459</v>
       </c>
       <c r="D8" t="n">
-        <v>498</v>
+        <v>878</v>
       </c>
       <c r="E8" t="n">
-        <v>2507</v>
+        <v>1203</v>
       </c>
       <c r="F8" t="n">
-        <v>16039</v>
+        <v>9993</v>
       </c>
       <c r="G8" t="n">
-        <v>14.49</v>
+        <v>10.2</v>
       </c>
       <c r="H8" t="n">
-        <v>2.28</v>
+        <v>13.66</v>
       </c>
       <c r="I8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J8" t="n">
         <v>9</v>
       </c>
       <c r="K8" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -745,25 +745,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>17098</v>
+        <v>16415</v>
       </c>
       <c r="C9" t="n">
-        <v>1228</v>
+        <v>136</v>
       </c>
       <c r="D9" t="n">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="E9" t="n">
-        <v>1161</v>
+        <v>566</v>
       </c>
       <c r="F9" t="n">
-        <v>14446</v>
+        <v>15433</v>
       </c>
       <c r="G9" t="n">
-        <v>18.17</v>
+        <v>18.86</v>
       </c>
       <c r="H9" t="n">
-        <v>14.9</v>
+        <v>5.6</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -772,7 +772,7 @@
         <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -782,34 +782,34 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>6422</v>
+        <v>2645</v>
       </c>
       <c r="C10" t="n">
-        <v>3460</v>
+        <v>886</v>
       </c>
       <c r="D10" t="n">
-        <v>403</v>
+        <v>370</v>
       </c>
       <c r="E10" t="n">
-        <v>2559</v>
+        <v>1389</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>10.34</v>
+        <v>4.69</v>
       </c>
       <c r="H10" t="n">
-        <v>4.44</v>
+        <v>3.36</v>
       </c>
       <c r="I10" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="J10" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K10" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -819,34 +819,34 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>14837</v>
+        <v>15789</v>
       </c>
       <c r="C11" t="n">
-        <v>303</v>
+        <v>563</v>
       </c>
       <c r="D11" t="n">
-        <v>299</v>
+        <v>247</v>
       </c>
       <c r="E11" t="n">
-        <v>213</v>
+        <v>696</v>
       </c>
       <c r="F11" t="n">
-        <v>14022</v>
+        <v>14283</v>
       </c>
       <c r="G11" t="n">
-        <v>17.82</v>
+        <v>8.43</v>
       </c>
       <c r="H11" t="n">
-        <v>3.97</v>
+        <v>8.140000000000001</v>
       </c>
       <c r="I11" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J11" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K11" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -856,34 +856,34 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>11030</v>
+        <v>8706</v>
       </c>
       <c r="C12" t="n">
-        <v>1675</v>
+        <v>1208</v>
       </c>
       <c r="D12" t="n">
-        <v>433</v>
+        <v>562</v>
       </c>
       <c r="E12" t="n">
-        <v>1648</v>
+        <v>1178</v>
       </c>
       <c r="F12" t="n">
-        <v>7273</v>
+        <v>5756</v>
       </c>
       <c r="G12" t="n">
-        <v>13.61</v>
+        <v>11.81</v>
       </c>
       <c r="H12" t="n">
-        <v>6.88</v>
+        <v>8.26</v>
       </c>
       <c r="I12" t="n">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="J12" t="n">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="K12" t="n">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13">
@@ -893,34 +893,34 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>15312</v>
+        <v>18114</v>
       </c>
       <c r="C13" t="n">
-        <v>514</v>
+        <v>357</v>
       </c>
       <c r="D13" t="n">
-        <v>526</v>
+        <v>704</v>
       </c>
       <c r="E13" t="n">
-        <v>876</v>
+        <v>1753</v>
       </c>
       <c r="F13" t="n">
-        <v>13395</v>
+        <v>15299</v>
       </c>
       <c r="G13" t="n">
-        <v>12.7</v>
+        <v>11.01</v>
       </c>
       <c r="H13" t="n">
-        <v>4.51</v>
+        <v>11.8</v>
       </c>
       <c r="I13" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J13" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="K13" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
@@ -930,25 +930,25 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>9167</v>
+        <v>18311</v>
       </c>
       <c r="C14" t="n">
-        <v>775</v>
+        <v>442</v>
       </c>
       <c r="D14" t="n">
-        <v>396</v>
+        <v>375</v>
       </c>
       <c r="E14" t="n">
-        <v>772</v>
+        <v>971</v>
       </c>
       <c r="F14" t="n">
-        <v>7223</v>
+        <v>16522</v>
       </c>
       <c r="G14" t="n">
-        <v>11.82</v>
+        <v>17.57</v>
       </c>
       <c r="H14" t="n">
-        <v>10.69</v>
+        <v>11.83</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
@@ -957,7 +957,7 @@
         <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
@@ -967,34 +967,34 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>12618</v>
+        <v>14599</v>
       </c>
       <c r="C15" t="n">
-        <v>1875</v>
+        <v>2857</v>
       </c>
       <c r="D15" t="n">
-        <v>697</v>
+        <v>636</v>
       </c>
       <c r="E15" t="n">
-        <v>411</v>
+        <v>3186</v>
       </c>
       <c r="F15" t="n">
-        <v>9635</v>
+        <v>7920</v>
       </c>
       <c r="G15" t="n">
-        <v>20.27</v>
+        <v>7.69</v>
       </c>
       <c r="H15" t="n">
-        <v>1.1</v>
+        <v>5.74</v>
       </c>
       <c r="I15" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K15" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1080,25 +1080,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19716</v>
+        <v>15356</v>
       </c>
       <c r="C2" t="n">
-        <v>568</v>
+        <v>2398</v>
       </c>
       <c r="D2" t="n">
-        <v>425</v>
+        <v>669</v>
       </c>
       <c r="E2" t="n">
-        <v>1111</v>
+        <v>894</v>
       </c>
       <c r="F2" t="n">
-        <v>17612</v>
+        <v>11395</v>
       </c>
       <c r="G2" t="n">
-        <v>13.48</v>
+        <v>27.85</v>
       </c>
       <c r="H2" t="n">
-        <v>15.68</v>
+        <v>9.67</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -1107,7 +1107,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -1117,34 +1117,34 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>13577</v>
+        <v>17551</v>
       </c>
       <c r="C3" t="n">
-        <v>2732</v>
+        <v>3395</v>
       </c>
       <c r="D3" t="n">
-        <v>636</v>
+        <v>1973</v>
       </c>
       <c r="E3" t="n">
-        <v>2326</v>
+        <v>1442</v>
       </c>
       <c r="F3" t="n">
-        <v>7883</v>
+        <v>10741</v>
       </c>
       <c r="G3" t="n">
-        <v>8.02</v>
+        <v>3.52</v>
       </c>
       <c r="H3" t="n">
-        <v>6.11</v>
+        <v>24.93</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K3" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -1154,34 +1154,34 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7823</v>
+        <v>13204</v>
       </c>
       <c r="C4" t="n">
-        <v>542</v>
+        <v>870</v>
       </c>
       <c r="D4" t="n">
-        <v>321</v>
+        <v>193</v>
       </c>
       <c r="E4" t="n">
-        <v>976</v>
+        <v>369</v>
       </c>
       <c r="F4" t="n">
-        <v>5984</v>
+        <v>11772</v>
       </c>
       <c r="G4" t="n">
-        <v>8.359999999999999</v>
+        <v>6.42</v>
       </c>
       <c r="H4" t="n">
-        <v>6.77</v>
+        <v>4.28</v>
       </c>
       <c r="I4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J4" t="n">
         <v>2</v>
       </c>
       <c r="K4" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
@@ -1191,28 +1191,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>25013</v>
+        <v>19823</v>
       </c>
       <c r="C5" t="n">
-        <v>187</v>
+        <v>1820</v>
       </c>
       <c r="D5" t="n">
-        <v>1342</v>
+        <v>917</v>
       </c>
       <c r="E5" t="n">
-        <v>2814</v>
+        <v>2963</v>
       </c>
       <c r="F5" t="n">
-        <v>20670</v>
+        <v>14123</v>
       </c>
       <c r="G5" t="n">
-        <v>20.68</v>
+        <v>3.95</v>
       </c>
       <c r="H5" t="n">
-        <v>21.73</v>
+        <v>9.57</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -1228,34 +1228,34 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>13541</v>
+        <v>11574</v>
       </c>
       <c r="C6" t="n">
-        <v>322</v>
+        <v>418</v>
       </c>
       <c r="D6" t="n">
-        <v>523</v>
+        <v>614</v>
       </c>
       <c r="E6" t="n">
-        <v>1751</v>
+        <v>3499</v>
       </c>
       <c r="F6" t="n">
-        <v>10945</v>
+        <v>7043</v>
       </c>
       <c r="G6" t="n">
-        <v>3.97</v>
+        <v>9.15</v>
       </c>
       <c r="H6" t="n">
-        <v>5.35</v>
+        <v>3.92</v>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J6" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K6" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -1265,34 +1265,34 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>10149</v>
+        <v>9131</v>
       </c>
       <c r="C7" t="n">
-        <v>2003</v>
+        <v>3026</v>
       </c>
       <c r="D7" t="n">
-        <v>726</v>
+        <v>672</v>
       </c>
       <c r="E7" t="n">
-        <v>1146</v>
+        <v>1370</v>
       </c>
       <c r="F7" t="n">
-        <v>6274</v>
+        <v>4063</v>
       </c>
       <c r="G7" t="n">
-        <v>24.02</v>
+        <v>3.18</v>
       </c>
       <c r="H7" t="n">
-        <v>8.869999999999999</v>
+        <v>1.84</v>
       </c>
       <c r="I7" t="n">
+        <v>19</v>
+      </c>
+      <c r="J7" t="n">
         <v>18</v>
       </c>
-      <c r="J7" t="n">
-        <v>13</v>
-      </c>
       <c r="K7" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -1302,34 +1302,34 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>13963</v>
+        <v>19179</v>
       </c>
       <c r="C8" t="n">
-        <v>1852</v>
+        <v>467</v>
       </c>
       <c r="D8" t="n">
-        <v>825</v>
+        <v>1579</v>
       </c>
       <c r="E8" t="n">
-        <v>1293</v>
+        <v>2255</v>
       </c>
       <c r="F8" t="n">
-        <v>9993</v>
+        <v>14878</v>
       </c>
       <c r="G8" t="n">
-        <v>9.880000000000001</v>
+        <v>16.52</v>
       </c>
       <c r="H8" t="n">
-        <v>13.37</v>
+        <v>6.99</v>
       </c>
       <c r="I8" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J8" t="n">
         <v>9</v>
       </c>
       <c r="K8" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
@@ -1339,25 +1339,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>16423</v>
+        <v>19363</v>
       </c>
       <c r="C9" t="n">
-        <v>127</v>
+        <v>718</v>
       </c>
       <c r="D9" t="n">
-        <v>313</v>
+        <v>725</v>
       </c>
       <c r="E9" t="n">
-        <v>622</v>
+        <v>259</v>
       </c>
       <c r="F9" t="n">
-        <v>15361</v>
+        <v>17661</v>
       </c>
       <c r="G9" t="n">
-        <v>18.86</v>
+        <v>9.029999999999999</v>
       </c>
       <c r="H9" t="n">
-        <v>5.6</v>
+        <v>5.67</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -1366,7 +1366,7 @@
         <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -1376,34 +1376,34 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2653</v>
+        <v>19287</v>
       </c>
       <c r="C10" t="n">
-        <v>894</v>
+        <v>1064</v>
       </c>
       <c r="D10" t="n">
-        <v>370</v>
+        <v>856</v>
       </c>
       <c r="E10" t="n">
-        <v>1389</v>
+        <v>596</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>16771</v>
       </c>
       <c r="G10" t="n">
-        <v>4.72</v>
+        <v>7.15</v>
       </c>
       <c r="H10" t="n">
-        <v>3.37</v>
+        <v>12.95</v>
       </c>
       <c r="I10" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="J10" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K10" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
@@ -1413,34 +1413,34 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>15789</v>
+        <v>6203</v>
       </c>
       <c r="C11" t="n">
-        <v>563</v>
+        <v>2297</v>
       </c>
       <c r="D11" t="n">
-        <v>247</v>
+        <v>446</v>
       </c>
       <c r="E11" t="n">
-        <v>696</v>
+        <v>564</v>
       </c>
       <c r="F11" t="n">
-        <v>14283</v>
+        <v>2896</v>
       </c>
       <c r="G11" t="n">
-        <v>13.42</v>
+        <v>10.82</v>
       </c>
       <c r="H11" t="n">
-        <v>12.94</v>
+        <v>9.380000000000001</v>
       </c>
       <c r="I11" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J11" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="K11" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1450,34 +1450,34 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>8647</v>
+        <v>15200</v>
       </c>
       <c r="C12" t="n">
-        <v>1322</v>
+        <v>1356</v>
       </c>
       <c r="D12" t="n">
-        <v>560</v>
+        <v>825</v>
       </c>
       <c r="E12" t="n">
-        <v>1201</v>
+        <v>1147</v>
       </c>
       <c r="F12" t="n">
-        <v>5562</v>
+        <v>11871</v>
       </c>
       <c r="G12" t="n">
-        <v>11.74</v>
+        <v>8.32</v>
       </c>
       <c r="H12" t="n">
-        <v>8.1</v>
+        <v>6.52</v>
       </c>
       <c r="I12" t="n">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="J12" t="n">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="K12" t="n">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13">
@@ -1487,34 +1487,34 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>18114</v>
+        <v>12533</v>
       </c>
       <c r="C13" t="n">
-        <v>357</v>
+        <v>1511</v>
       </c>
       <c r="D13" t="n">
-        <v>704</v>
+        <v>659</v>
       </c>
       <c r="E13" t="n">
-        <v>1753</v>
+        <v>2342</v>
       </c>
       <c r="F13" t="n">
-        <v>15299</v>
+        <v>8020</v>
       </c>
       <c r="G13" t="n">
-        <v>12.69</v>
+        <v>7.97</v>
       </c>
       <c r="H13" t="n">
-        <v>13.34</v>
+        <v>7.62</v>
       </c>
       <c r="I13" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="J13" t="n">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="K13" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14">
@@ -1524,25 +1524,25 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>18069</v>
+        <v>17359</v>
       </c>
       <c r="C14" t="n">
-        <v>347</v>
+        <v>1558</v>
       </c>
       <c r="D14" t="n">
-        <v>369</v>
+        <v>697</v>
       </c>
       <c r="E14" t="n">
-        <v>866</v>
+        <v>576</v>
       </c>
       <c r="F14" t="n">
-        <v>16486</v>
+        <v>14528</v>
       </c>
       <c r="G14" t="n">
-        <v>16.17</v>
+        <v>18.44</v>
       </c>
       <c r="H14" t="n">
-        <v>10.64</v>
+        <v>7.66</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
@@ -1551,7 +1551,7 @@
         <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -1561,34 +1561,34 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>13577</v>
+        <v>17551</v>
       </c>
       <c r="C15" t="n">
-        <v>2732</v>
+        <v>3395</v>
       </c>
       <c r="D15" t="n">
-        <v>636</v>
+        <v>1973</v>
       </c>
       <c r="E15" t="n">
-        <v>2326</v>
+        <v>1442</v>
       </c>
       <c r="F15" t="n">
-        <v>7883</v>
+        <v>10741</v>
       </c>
       <c r="G15" t="n">
-        <v>8.02</v>
+        <v>3.52</v>
       </c>
       <c r="H15" t="n">
-        <v>6.1</v>
+        <v>24.93</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K15" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>